<commit_message>
MARP-637: update unit test
</commit_message>
<xml_diff>
--- a/excel-importer-test/src_test/com/axonivy/util/excel/test/sample.xlsx
+++ b/excel-importer-test/src_test/com/axonivy/util/excel/test/sample.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Firstname</t>
   </si>
@@ -56,6 +56,15 @@
     <t>Note</t>
   </si>
   <si>
+    <t>Wrong number format with dot should be String</t>
+  </si>
+  <si>
+    <t>Wrong number format with comma should be String</t>
+  </si>
+  <si>
+    <t>Column contains number should be String</t>
+  </si>
+  <si>
     <t>Hugo</t>
   </si>
   <si>
@@ -87,6 +96,15 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>15024.00.00</t>
+  </si>
+  <si>
+    <t>15024,00,00</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum</t>
   </si>
 </sst>
 </file>
@@ -702,12 +720,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1241,10 +1260,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.552380952381" defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -1253,10 +1272,13 @@
     <col min="5" max="5" width="11.5238095238095" style="1"/>
     <col min="6" max="6" width="11.5238095238095" style="2"/>
     <col min="7" max="7" width="11.5428571428571" style="3"/>
-    <col min="9" max="9" width="28.1428571428571" customWidth="1"/>
+    <col min="9" max="9" width="74.7142857142857" customWidth="1"/>
+    <col min="10" max="10" width="42.4285714285714" customWidth="1"/>
+    <col min="11" max="11" width="48.2857142857143" customWidth="1"/>
+    <col min="12" max="12" width="49.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1284,25 +1306,34 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D2" s="4">
         <v>6300</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G2" s="3">
         <v>33193</v>
@@ -1311,33 +1342,51 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>123</v>
+      </c>
+      <c r="L2" s="5">
+        <v>123412341231</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4">
         <v>6210</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3">
         <v>33955</v>
       </c>
       <c r="H3">
         <v>1.2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MARP-637: Cells with "wrong" numbers should not be reconized as numbers (#59)
* MARP-637: Fix column with both string and numeric types

* MARP-637: Handle feedback

* MARP-637: update unit test

* MARP-637: handle feedback

* MARP-637: handle feedback
</commit_message>
<xml_diff>
--- a/excel-importer-test/src_test/com/axonivy/util/excel/test/sample.xlsx
+++ b/excel-importer-test/src_test/com/axonivy/util/excel/test/sample.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Firstname</t>
   </si>
@@ -56,6 +56,12 @@
     <t>Note</t>
   </si>
   <si>
+    <t>Column contains texts in incorrect number format</t>
+  </si>
+  <si>
+    <t>Column contains both text and numeric</t>
+  </si>
+  <si>
     <t>Hugo</t>
   </si>
   <si>
@@ -74,6 +80,9 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Quisque ut lacus a dui cursus aliquet. Phasellus eget semper libero, ac pharetra justo. Duis sit amet nisl id lorem malesuada cursus. Integer finibus, lacus sed accumsan tincidunt, nisl eros tincidunt ex, et suscipit justo libero id ante. Donec euismod bibendum vehicula. Curabitur bibendum, urna nec ultrices facilisis, orci mi tincidunt velit, at feugiat lorem ligula a urna. Sed tincidunt auctor mauris, sed cursus lacus. Cras vel nisi quam. Suspendisse potenti. Aenean quis vehicula est. Vivamus scelerisque eros ac sollicitudin consectetur. Donec id vulputate turpis. Praesent luctus, est nec fermentum cursus, velit neque sollicitudin velit, vitae ultricies sapien nunc id leo. Proin venenatis tristique tincidunt. Integer scelerisque ultricies ex.</t>
   </si>
   <si>
+    <t>401491.00.00</t>
+  </si>
+  <si>
     <t>Fritz</t>
   </si>
   <si>
@@ -87,6 +96,12 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>3100310.00.00</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum</t>
   </si>
 </sst>
 </file>
@@ -702,12 +717,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1241,10 +1257,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.552380952381" defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -1253,10 +1269,12 @@
     <col min="5" max="5" width="11.5238095238095" style="1"/>
     <col min="6" max="6" width="11.5238095238095" style="2"/>
     <col min="7" max="7" width="11.5428571428571" style="3"/>
-    <col min="9" max="9" width="28.1428571428571" customWidth="1"/>
+    <col min="9" max="9" width="68.7142857142857" customWidth="1"/>
+    <col min="10" max="10" width="52.2857142857143" customWidth="1"/>
+    <col min="11" max="11" width="49.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1284,25 +1302,31 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4">
         <v>6300</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" s="3">
         <v>33193</v>
@@ -1311,33 +1335,45 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="5">
+        <v>1234121</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4">
         <v>6210</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3">
         <v>33955</v>
       </c>
       <c r="H3">
         <v>1.2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>